<commit_message>
Fixed erasing. Moved the button
</commit_message>
<xml_diff>
--- a/BedsPlan/BedsPlan.xlsx
+++ b/BedsPlan/BedsPlan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16725" windowHeight="4680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23610" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ResultTemplate" sheetId="3" r:id="rId1"/>
@@ -779,36 +779,19 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4A5B185774D4C644D5B49C69418967FF8CC444"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1F0C583D81DEED142B9198CA1311A549F9BB31"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="5821"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="873"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1111"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="36B26063B3EBEA3459D3B8BD3D48F181BF1D33"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="6165"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1111"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -825,18 +808,35 @@
 </ax:ocx>
 </file>
 
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4A5B185774D4C644D5B49C69418967FF8CC444"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4260"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1058"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1F0C583D81DEED142B9198CA1311A549F9BB31"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="153B24F7E169C7144FB1843010F77CAD9B18D1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="6165"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="1111"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
@@ -967,22 +967,86 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>914400</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>0</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>723900</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>590550</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>400050</xdr:rowOff>
+          <xdr:rowOff>381000</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="_ActiveXWrapper3" hidden="1">
+            <xdr:cNvPr id="1028" name="_ActiveXWrapper4" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>66675</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>457200</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3073" name="_ActiveXWrapper1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1013,76 +1077,6 @@
                   <a:headEnd/>
                   <a:tailEnd/>
                 </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>1171574</xdr:colOff>
-          <xdr:row>0</xdr:row>
-          <xdr:rowOff>352425</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="_ActiveXWrapper4" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1028"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:prstDash val="solid"/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd type="none" w="med" len="med"/>
-                </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -1629,7 +1623,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,43 +1777,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId4" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="1025" r:id="rId4" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>1171575</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>352425</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId4" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId6" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>914400</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>723900</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>1171575</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>400050</xdr:rowOff>
               </to>
@@ -1828,13 +1797,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId6" name="_ActiveXWrapper3"/>
+        <control shapeId="1025" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId8" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="1026" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -1853,32 +1822,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId8" name="_ActiveXWrapper2"/>
+        <control shapeId="1026" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId10" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+        <control shapeId="1028" r:id="rId8" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>1171575</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>590550</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>400050</xdr:rowOff>
+                <xdr:rowOff>381000</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId10" name="_ActiveXWrapper1"/>
+        <control shapeId="1028" r:id="rId8" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -1886,17 +1855,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист5"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3073" r:id="rId4" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3073" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 

</xml_diff>